<commit_message>
Adding BDD method for login case
</commit_message>
<xml_diff>
--- a/Data Files/loginInvalidData.xlsx
+++ b/Data Files/loginInvalidData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Binar\Training\Katalon\Magento\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E85DD-66F0-474B-BCFD-49A7C13E7004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F97304E-A3F0-4BB2-B1DC-687FE07184D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4D41FBA2-2527-437E-8BA9-450530EC50F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>userMail</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Please enter a valid email address (Ex: johndoe@domain.com).</t>
+  </si>
+  <si>
+    <t>salah.Passwd</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC8D103-BEC4-42AF-A04B-790E449A6964}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,6 +502,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>